<commit_message>
fix navbar & banner
</commit_message>
<xml_diff>
--- a/template_task.xlsx
+++ b/template_task.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\1CyberSoft\FileBaiTap\BC10\BC10-TanPhong-Capstone-Dinner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC362F8F-CF7B-494B-9A49-7D9855CAF53A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB08155C-B730-48E6-AE72-5E918078B8C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
   <si>
     <t>Tasks Name</t>
   </si>
@@ -72,9 +72,6 @@
   </si>
   <si>
     <t>Header</t>
-  </si>
-  <si>
-    <t>12/13</t>
   </si>
   <si>
     <t xml:space="preserve">     Logo</t>
@@ -135,8 +132,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="mm/dd"/>
+    <numFmt numFmtId="167" formatCode="m/d;@"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -350,9 +348,6 @@
     <xf numFmtId="164" fontId="2" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="9" fontId="3" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -387,6 +382,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="2" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -632,7 +630,7 @@
   <dimension ref="A1:J986"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" outlineLevelRow="2" x14ac:dyDescent="0.2"/>
@@ -687,46 +685,48 @@
       <c r="B2" s="8">
         <v>45268</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="10"/>
-      <c r="E2" s="11" t="s">
-        <v>27</v>
+      <c r="C2" s="22">
+        <v>45271</v>
+      </c>
+      <c r="D2" s="9">
+        <v>0.9</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>26</v>
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="13"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="12"/>
     </row>
     <row r="3" spans="1:10" ht="14.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="14" t="s">
-        <v>11</v>
+      <c r="A3" s="13" t="s">
+        <v>10</v>
       </c>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
-      <c r="D3" s="15">
+      <c r="D3" s="14">
         <v>0.5</v>
       </c>
-      <c r="E3" s="11" t="s">
-        <v>12</v>
+      <c r="E3" s="10" t="s">
+        <v>11</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="8">
         <v>44179</v>
       </c>
-      <c r="H3" s="16">
+      <c r="H3" s="15">
         <v>0.5</v>
       </c>
-      <c r="I3" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="J3" s="13"/>
+      <c r="I3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="12"/>
     </row>
     <row r="4" spans="1:10" ht="14.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="8">
         <v>43608</v>
@@ -734,269 +734,273 @@
       <c r="C4" s="8">
         <v>43647</v>
       </c>
-      <c r="D4" s="17">
+      <c r="D4" s="16">
         <f>SUM(D5:D7)/3</f>
         <v>0.9</v>
       </c>
-      <c r="E4" s="11" t="s">
-        <v>12</v>
+      <c r="E4" s="10" t="s">
+        <v>11</v>
       </c>
       <c r="F4" s="8"/>
       <c r="G4" s="8">
         <v>44179</v>
       </c>
-      <c r="H4" s="18">
+      <c r="H4" s="17">
         <f>SUM(H5:H7)/3</f>
         <v>0.9</v>
       </c>
-      <c r="I4" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="J4" s="13"/>
+      <c r="I4" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="12"/>
     </row>
     <row r="5" spans="1:10" ht="14.25" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
-      <c r="A5" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="19">
+      <c r="A5" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="18">
         <v>43608</v>
       </c>
-      <c r="C5" s="19">
+      <c r="C5" s="18">
         <v>43616</v>
       </c>
-      <c r="D5" s="17">
+      <c r="D5" s="16">
         <v>1</v>
       </c>
-      <c r="E5" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="19"/>
+      <c r="E5" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="18"/>
       <c r="G5" s="8">
         <v>44179</v>
       </c>
-      <c r="H5" s="18">
+      <c r="H5" s="17">
         <v>1</v>
       </c>
-      <c r="I5" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="J5" s="13"/>
+      <c r="I5" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" s="12"/>
     </row>
     <row r="6" spans="1:10" ht="14.25" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
-      <c r="A6" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="19">
+      <c r="A6" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="18">
         <v>43636</v>
       </c>
-      <c r="C6" s="19">
+      <c r="C6" s="18">
         <v>43644</v>
       </c>
-      <c r="D6" s="17">
+      <c r="D6" s="16">
         <v>0.9</v>
       </c>
-      <c r="E6" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="19"/>
+      <c r="E6" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="18"/>
       <c r="G6" s="8">
         <v>44179</v>
       </c>
-      <c r="H6" s="18">
+      <c r="H6" s="17">
         <v>0.9</v>
       </c>
-      <c r="I6" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="J6" s="13"/>
+      <c r="I6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J6" s="12"/>
     </row>
     <row r="7" spans="1:10" ht="9" hidden="1" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.2">
-      <c r="A7" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="19">
+      <c r="A7" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="18">
         <v>43641</v>
       </c>
-      <c r="C7" s="19">
+      <c r="C7" s="18">
         <v>43647</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7" s="16">
         <v>0.8</v>
       </c>
-      <c r="E7" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="19"/>
+      <c r="E7" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="18"/>
       <c r="G7" s="8">
         <v>44179</v>
       </c>
-      <c r="H7" s="18">
+      <c r="H7" s="17">
         <v>0.8</v>
       </c>
-      <c r="I7" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="J7" s="20"/>
+      <c r="I7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J7" s="19"/>
     </row>
     <row r="8" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" s="8">
         <v>45268</v>
       </c>
       <c r="C8" s="8">
-        <v>44178</v>
-      </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="11" t="s">
-        <v>27</v>
+        <v>44176</v>
+      </c>
+      <c r="D8" s="9">
+        <v>0.9</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>26</v>
       </c>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="13"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="12"/>
     </row>
     <row r="9" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="11" t="s">
-        <v>28</v>
+      <c r="D9" s="9"/>
+      <c r="E9" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="13"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="12"/>
     </row>
     <row r="10" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="8"/>
+        <v>19</v>
+      </c>
+      <c r="B10" s="8">
+        <v>45271</v>
+      </c>
       <c r="C10" s="8"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="11" t="s">
-        <v>27</v>
+      <c r="D10" s="9"/>
+      <c r="E10" s="10" t="s">
+        <v>26</v>
       </c>
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="13"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="12"/>
     </row>
     <row r="11" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="11" t="s">
-        <v>28</v>
+      <c r="D11" s="9"/>
+      <c r="E11" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="13"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="12"/>
     </row>
     <row r="12" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="21" t="s">
-        <v>28</v>
+      <c r="D12" s="9"/>
+      <c r="E12" s="20" t="s">
+        <v>27</v>
       </c>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="13"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="12"/>
     </row>
     <row r="13" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="22" t="s">
-        <v>28</v>
+      <c r="D13" s="9"/>
+      <c r="E13" s="21" t="s">
+        <v>27</v>
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="13"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="12"/>
     </row>
     <row r="14" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="11" t="s">
-        <v>27</v>
+      <c r="D14" s="9"/>
+      <c r="E14" s="10" t="s">
+        <v>26</v>
       </c>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="13"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="12"/>
     </row>
     <row r="15" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="22" t="s">
-        <v>27</v>
+      <c r="D15" s="9"/>
+      <c r="E15" s="21" t="s">
+        <v>26</v>
       </c>
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="13"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="12"/>
     </row>
     <row r="16" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="11" t="s">
-        <v>28</v>
+      <c r="D16" s="9"/>
+      <c r="E16" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="13"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="12"/>
     </row>
     <row r="17" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="22"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="21"/>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="13"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="12"/>
     </row>
     <row r="18" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="19" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>